<commit_message>
update LCP matrix by keeping only regions used for Fst
</commit_message>
<xml_diff>
--- a/00_Data/00_fileinfo/AI_LCP_Distance.xlsx
+++ b/00_Data/00_fileinfo/AI_LCP_Distance.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\GitHub\NA_AerInsect_LandscapeGenomics\00_Data\00_fileinfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\GitHub\NA_AerialInsectivores_LandGeno\00_Data\00_fileinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514AF9D6-05E6-4849-90B4-EFDA890EC611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0BB0B4-9E85-402C-A8C5-CCB53C0B7B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{EC123050-981E-4163-BD10-4CED8A994C48}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{EC123050-981E-4163-BD10-4CED8A994C48}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALFL_LCP_Distance_2" sheetId="6" r:id="rId1"/>
-    <sheet name="ALFL_LCP_Distance" sheetId="1" r:id="rId2"/>
+    <sheet name="ALFL_LCP_Distance" sheetId="1" r:id="rId1"/>
+    <sheet name="ALFL_LCP_Distance_2" sheetId="6" r:id="rId2"/>
     <sheet name="CLSW_LCP_Distance" sheetId="2" r:id="rId3"/>
-    <sheet name="PUMA_LCP_Distance_2" sheetId="8" r:id="rId4"/>
-    <sheet name="PUMA_LCP_Distance" sheetId="3" r:id="rId5"/>
-    <sheet name="VGSW_LCP_Distance_2" sheetId="9" r:id="rId6"/>
-    <sheet name="VGSW_LCP_Distance" sheetId="4" r:id="rId7"/>
+    <sheet name="PUMA_LCP_Distance" sheetId="3" r:id="rId4"/>
+    <sheet name="PUMA_LCP_Distance_2" sheetId="8" r:id="rId5"/>
+    <sheet name="VGSW_LCP_Distance" sheetId="4" r:id="rId6"/>
+    <sheet name="VGSW_LCP_Distance_2" sheetId="9" r:id="rId7"/>
     <sheet name="Read_Me" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="28">
   <si>
     <t>LCP distance</t>
   </si>
@@ -513,6 +513,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C25153D-5F21-4E0B-8BAA-0926C00B1C12}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>5606816.2009498803</v>
+      </c>
+      <c r="D2">
+        <v>5845621.6716127396</v>
+      </c>
+      <c r="E2">
+        <v>3602820.2232679301</v>
+      </c>
+      <c r="F2">
+        <v>999194.23811189795</v>
+      </c>
+      <c r="G2">
+        <v>975388.20746252802</v>
+      </c>
+      <c r="H2">
+        <v>5174378.4438734697</v>
+      </c>
+      <c r="I2">
+        <v>463523.19940226403</v>
+      </c>
+      <c r="J2">
+        <v>1439281.7312099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5606816.2009498803</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>329765.41262629401</v>
+      </c>
+      <c r="E3">
+        <v>2375205.0129657099</v>
+      </c>
+      <c r="F3">
+        <v>5548845.9593195198</v>
+      </c>
+      <c r="G3">
+        <v>6312721.0392405801</v>
+      </c>
+      <c r="H3">
+        <v>6911700.2537780898</v>
+      </c>
+      <c r="I3">
+        <v>5140240.5510333199</v>
+      </c>
+      <c r="J3">
+        <v>6923259.2628985504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5845621.6716127396</v>
+      </c>
+      <c r="C4">
+        <v>329765.41262629401</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2614010.4836285701</v>
+      </c>
+      <c r="F4">
+        <v>5787651.4299823698</v>
+      </c>
+      <c r="G4">
+        <v>6551526.50990343</v>
+      </c>
+      <c r="H4">
+        <v>7150505.7244409397</v>
+      </c>
+      <c r="I4">
+        <v>5379046.0216961801</v>
+      </c>
+      <c r="J4">
+        <v>7162064.7335614003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3602820.2232679301</v>
+      </c>
+      <c r="C5">
+        <v>2375205.0129657099</v>
+      </c>
+      <c r="D5">
+        <v>2614010.4836285701</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>3544849.9816375701</v>
+      </c>
+      <c r="G5">
+        <v>4308725.0615586396</v>
+      </c>
+      <c r="H5">
+        <v>4620175.7710992899</v>
+      </c>
+      <c r="I5">
+        <v>3136244.5733514</v>
+      </c>
+      <c r="J5">
+        <v>4919263.2852166099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>999194.23811189795</v>
+      </c>
+      <c r="C6">
+        <v>5548845.9593195198</v>
+      </c>
+      <c r="D6">
+        <v>5787651.4299823698</v>
+      </c>
+      <c r="E6">
+        <v>3544849.9816375701</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1100729.2913858199</v>
+      </c>
+      <c r="H6">
+        <v>5198824.3661285704</v>
+      </c>
+      <c r="I6">
+        <v>1003817.84176009</v>
+      </c>
+      <c r="J6">
+        <v>1945909.5621571401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>975388.20746252802</v>
+      </c>
+      <c r="C7">
+        <v>6312721.0392405801</v>
+      </c>
+      <c r="D7">
+        <v>6551526.50990343</v>
+      </c>
+      <c r="E7">
+        <v>4308725.0615586396</v>
+      </c>
+      <c r="F7">
+        <v>1100729.2913858199</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>5962699.4460496297</v>
+      </c>
+      <c r="I7">
+        <v>1312893.2118639499</v>
+      </c>
+      <c r="J7">
+        <v>992872.40610447002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5174378.4438734697</v>
+      </c>
+      <c r="C8">
+        <v>6911700.2537780898</v>
+      </c>
+      <c r="D8">
+        <v>7150505.7244409397</v>
+      </c>
+      <c r="E8">
+        <v>4620175.7710992899</v>
+      </c>
+      <c r="F8">
+        <v>5198824.3661285704</v>
+      </c>
+      <c r="G8">
+        <v>5962699.4460496297</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>4505997.0538104698</v>
+      </c>
+      <c r="J8">
+        <v>6573237.6697075898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>463523.19940226403</v>
+      </c>
+      <c r="C9">
+        <v>5140240.5510333199</v>
+      </c>
+      <c r="D9">
+        <v>5379046.0216961801</v>
+      </c>
+      <c r="E9">
+        <v>3136244.5733514</v>
+      </c>
+      <c r="F9">
+        <v>1003817.84176009</v>
+      </c>
+      <c r="G9">
+        <v>1312893.2118639499</v>
+      </c>
+      <c r="H9">
+        <v>4505997.0538104698</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1923431.43552192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1439281.7312099</v>
+      </c>
+      <c r="C10">
+        <v>6923259.2628985504</v>
+      </c>
+      <c r="D10">
+        <v>7162064.7335614003</v>
+      </c>
+      <c r="E10">
+        <v>4919263.2852166099</v>
+      </c>
+      <c r="F10">
+        <v>1945909.5621571401</v>
+      </c>
+      <c r="G10">
+        <v>992872.40610447002</v>
+      </c>
+      <c r="H10">
+        <v>6573237.6697075898</v>
+      </c>
+      <c r="I10">
+        <v>1923431.43552192</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF39746-83BD-4768-A4DD-29A8A8F635CA}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -578,344 +916,6 @@
         <v>1312893.2118639499</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C25153D-5F21-4E0B-8BAA-0926C00B1C12}">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>5606816.2009498803</v>
-      </c>
-      <c r="D2">
-        <v>5845621.6716127396</v>
-      </c>
-      <c r="E2">
-        <v>3602820.2232679301</v>
-      </c>
-      <c r="F2">
-        <v>999194.23811189795</v>
-      </c>
-      <c r="G2">
-        <v>975388.20746252802</v>
-      </c>
-      <c r="H2">
-        <v>5174378.4438734697</v>
-      </c>
-      <c r="I2">
-        <v>463523.19940226403</v>
-      </c>
-      <c r="J2">
-        <v>1439281.7312099</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>5606816.2009498803</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>329765.41262629401</v>
-      </c>
-      <c r="E3">
-        <v>2375205.0129657099</v>
-      </c>
-      <c r="F3">
-        <v>5548845.9593195198</v>
-      </c>
-      <c r="G3">
-        <v>6312721.0392405801</v>
-      </c>
-      <c r="H3">
-        <v>6911700.2537780898</v>
-      </c>
-      <c r="I3">
-        <v>5140240.5510333199</v>
-      </c>
-      <c r="J3">
-        <v>6923259.2628985504</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>5845621.6716127396</v>
-      </c>
-      <c r="C4">
-        <v>329765.41262629401</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2614010.4836285701</v>
-      </c>
-      <c r="F4">
-        <v>5787651.4299823698</v>
-      </c>
-      <c r="G4">
-        <v>6551526.50990343</v>
-      </c>
-      <c r="H4">
-        <v>7150505.7244409397</v>
-      </c>
-      <c r="I4">
-        <v>5379046.0216961801</v>
-      </c>
-      <c r="J4">
-        <v>7162064.7335614003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>3602820.2232679301</v>
-      </c>
-      <c r="C5">
-        <v>2375205.0129657099</v>
-      </c>
-      <c r="D5">
-        <v>2614010.4836285701</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>3544849.9816375701</v>
-      </c>
-      <c r="G5">
-        <v>4308725.0615586396</v>
-      </c>
-      <c r="H5">
-        <v>4620175.7710992899</v>
-      </c>
-      <c r="I5">
-        <v>3136244.5733514</v>
-      </c>
-      <c r="J5">
-        <v>4919263.2852166099</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>999194.23811189795</v>
-      </c>
-      <c r="C6">
-        <v>5548845.9593195198</v>
-      </c>
-      <c r="D6">
-        <v>5787651.4299823698</v>
-      </c>
-      <c r="E6">
-        <v>3544849.9816375701</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1100729.2913858199</v>
-      </c>
-      <c r="H6">
-        <v>5198824.3661285704</v>
-      </c>
-      <c r="I6">
-        <v>1003817.84176009</v>
-      </c>
-      <c r="J6">
-        <v>1945909.5621571401</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>975388.20746252802</v>
-      </c>
-      <c r="C7">
-        <v>6312721.0392405801</v>
-      </c>
-      <c r="D7">
-        <v>6551526.50990343</v>
-      </c>
-      <c r="E7">
-        <v>4308725.0615586396</v>
-      </c>
-      <c r="F7">
-        <v>1100729.2913858199</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>5962699.4460496297</v>
-      </c>
-      <c r="I7">
-        <v>1312893.2118639499</v>
-      </c>
-      <c r="J7">
-        <v>992872.40610447002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>5174378.4438734697</v>
-      </c>
-      <c r="C8">
-        <v>6911700.2537780898</v>
-      </c>
-      <c r="D8">
-        <v>7150505.7244409397</v>
-      </c>
-      <c r="E8">
-        <v>4620175.7710992899</v>
-      </c>
-      <c r="F8">
-        <v>5198824.3661285704</v>
-      </c>
-      <c r="G8">
-        <v>5962699.4460496297</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>4505997.0538104698</v>
-      </c>
-      <c r="J8">
-        <v>6573237.6697075898</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>463523.19940226403</v>
-      </c>
-      <c r="C9">
-        <v>5140240.5510333199</v>
-      </c>
-      <c r="D9">
-        <v>5379046.0216961801</v>
-      </c>
-      <c r="E9">
-        <v>3136244.5733514</v>
-      </c>
-      <c r="F9">
-        <v>1003817.84176009</v>
-      </c>
-      <c r="G9">
-        <v>1312893.2118639499</v>
-      </c>
-      <c r="H9">
-        <v>4505997.0538104698</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>1923431.43552192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1439281.7312099</v>
-      </c>
-      <c r="C10">
-        <v>6923259.2628985504</v>
-      </c>
-      <c r="D10">
-        <v>7162064.7335614003</v>
-      </c>
-      <c r="E10">
-        <v>4919263.2852166099</v>
-      </c>
-      <c r="F10">
-        <v>1945909.5621571401</v>
-      </c>
-      <c r="G10">
-        <v>992872.40610447002</v>
-      </c>
-      <c r="H10">
-        <v>6573237.6697075898</v>
-      </c>
-      <c r="I10">
-        <v>1923431.43552192</v>
-      </c>
-      <c r="J10">
         <v>0</v>
       </c>
     </row>
@@ -1263,149 +1263,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DB9495-4F5F-4280-851F-E51C2896F235}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>3153797.3291031201</v>
-      </c>
-      <c r="D2">
-        <v>876392.54094215296</v>
-      </c>
-      <c r="E2">
-        <v>4263349.5296472404</v>
-      </c>
-      <c r="F2">
-        <v>4250197.4152147202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>3153797.3291031201</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>2530242.0552912601</v>
-      </c>
-      <c r="E3">
-        <v>1310614.5736974999</v>
-      </c>
-      <c r="F3">
-        <v>1297462.4592649799</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>876392.54094215296</v>
-      </c>
-      <c r="C4">
-        <v>2530242.0552912601</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>3639794.2558353902</v>
-      </c>
-      <c r="F4">
-        <v>3626642.1414028602</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>4263349.5296472404</v>
-      </c>
-      <c r="C5">
-        <v>1310614.5736974999</v>
-      </c>
-      <c r="D5">
-        <v>3639794.2558353902</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>213380.92383270501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>4250197.4152147202</v>
-      </c>
-      <c r="C6">
-        <v>1297462.4592649799</v>
-      </c>
-      <c r="D6">
-        <v>3626642.1414028602</v>
-      </c>
-      <c r="E6">
-        <v>213380.92383270501</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2F6E45-C0E5-4113-B5BB-29F4F89D31C1}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1679,12 +1541,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF86EB26-05A1-4B31-B4D5-FCCEEAA4E7E1}">
-  <dimension ref="A1:F6"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DB9495-4F5F-4280-851F-E51C2896F235}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1692,123 +1554,89 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>840122.80516532203</v>
+        <v>4263349.5296472404</v>
       </c>
       <c r="D2">
-        <v>1700755.9413459499</v>
+        <v>3153797.3291031201</v>
       </c>
       <c r="E2">
-        <v>1617382.1977914299</v>
-      </c>
-      <c r="F2">
-        <v>1574214.0286338001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>876392.54094215296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>840122.80516532203</v>
+        <v>4263349.5296472404</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1797106.45378865</v>
+        <v>1310614.5736974999</v>
       </c>
       <c r="E3">
-        <v>1841322.0583688801</v>
-      </c>
-      <c r="F3">
-        <v>1574980.99546488</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3639794.2558353902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>1700755.9413459499</v>
+        <v>3153797.3291031201</v>
       </c>
       <c r="C4">
-        <v>1797106.45378865</v>
+        <v>1310614.5736974999</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>130118.08093772399</v>
-      </c>
-      <c r="F4">
-        <v>228230.35935232701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2530242.0552912601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>1617382.1977914299</v>
+        <v>876392.54094215296</v>
       </c>
       <c r="C5">
-        <v>1841322.0583688801</v>
+        <v>3639794.2558353902</v>
       </c>
       <c r="D5">
-        <v>130118.08093772399</v>
+        <v>2530242.0552912601</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>272445.963932566</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>1574214.0286338001</v>
-      </c>
-      <c r="C6">
-        <v>1574980.99546488</v>
-      </c>
-      <c r="D6">
-        <v>228230.35935232701</v>
-      </c>
-      <c r="E6">
-        <v>272445.963932566</v>
-      </c>
-      <c r="F6">
         <v>0</v>
       </c>
     </row>
@@ -1817,12 +1645,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3205CA70-3C17-411F-A34B-B09DF74465D3}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1988,6 +1816,144 @@
         <v>272445.963932566</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF86EB26-05A1-4B31-B4D5-FCCEEAA4E7E1}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>840122.80516532203</v>
+      </c>
+      <c r="D2">
+        <v>1700755.9413459499</v>
+      </c>
+      <c r="E2">
+        <v>1617382.1977914299</v>
+      </c>
+      <c r="F2">
+        <v>1574214.0286338001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>840122.80516532203</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1797106.45378865</v>
+      </c>
+      <c r="E3">
+        <v>1841322.0583688801</v>
+      </c>
+      <c r="F3">
+        <v>1574980.99546488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>1700755.9413459499</v>
+      </c>
+      <c r="C4">
+        <v>1797106.45378865</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>130118.08093772399</v>
+      </c>
+      <c r="F4">
+        <v>228230.35935232701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1617382.1977914299</v>
+      </c>
+      <c r="C5">
+        <v>1841322.0583688801</v>
+      </c>
+      <c r="D5">
+        <v>130118.08093772399</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>272445.963932566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>1574214.0286338001</v>
+      </c>
+      <c r="C6">
+        <v>1574980.99546488</v>
+      </c>
+      <c r="D6">
+        <v>228230.35935232701</v>
+      </c>
+      <c r="E6">
+        <v>272445.963932566</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
     </row>

</xml_diff>